<commit_message>
Add Notification for R7&R8 of USBPipe
</commit_message>
<xml_diff>
--- a/PCB/USBpipe/BOM_USBpipe_Rev1.x.xlsx
+++ b/PCB/USBpipe/BOM_USBpipe_Rev1.x.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lithium\Documents\GitHub\USBvalve\PCB\USBpipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45DDF59C-1A07-4CC3-97DB-A8A5D1B311E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3206019C-601D-465A-9E69-A931CCCB88AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6870" yWindow="2985" windowWidth="21600" windowHeight="11295"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_USBValve_Tagless_USB ValveT" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="75">
   <si>
     <t>No.</t>
   </si>
@@ -248,12 +248,18 @@
   <si>
     <t>Manufacturer</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOTE: R7 and R8 aren't actually connected to anything. They are added for circuit debugging purposes.</t>
+  </si>
+  <si>
+    <t>注意: R7和R8为测试用焊盘,并不连接到任何元件</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1198,11 +1204,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1709,6 +1715,16 @@
         <v>63</v>
       </c>
     </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix Document Mistake(#50) (#51)
* Add Notification for R7&R8 of USBPipe

* Document improvements
</commit_message>
<xml_diff>
--- a/PCB/USBpipe/BOM_USBpipe_Rev1.x.xlsx
+++ b/PCB/USBpipe/BOM_USBpipe_Rev1.x.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lithium\Documents\GitHub\USBvalve\PCB\USBpipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45DDF59C-1A07-4CC3-97DB-A8A5D1B311E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3206019C-601D-465A-9E69-A931CCCB88AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6870" yWindow="2985" windowWidth="21600" windowHeight="11295"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_USBValve_Tagless_USB ValveT" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="75">
   <si>
     <t>No.</t>
   </si>
@@ -248,12 +248,18 @@
   <si>
     <t>Manufacturer</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOTE: R7 and R8 aren't actually connected to anything. They are added for circuit debugging purposes.</t>
+  </si>
+  <si>
+    <t>注意: R7和R8为测试用焊盘,并不连接到任何元件</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1198,11 +1204,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1709,6 +1715,16 @@
         <v>63</v>
       </c>
     </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>